<commit_message>
tuned performance of the models
</commit_message>
<xml_diff>
--- a/v2-Implementation/Data/Optimal-Betas-complex-newcost.xlsx
+++ b/v2-Implementation/Data/Optimal-Betas-complex-newcost.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-59114.22063088336</v>
+        <v>-59114.2206308836</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>9.051792499119539</v>
+        <v>9.0517924991196</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>8.061792499119548</v>
+        <v>8.061792499119552</v>
       </c>
     </row>
     <row r="3">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>9.051792499119536</v>
+        <v>9.051792499119635</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>8.061792499119491</v>
+        <v>8.061792499119679</v>
       </c>
     </row>
     <row r="4">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>9.051792499119543</v>
+        <v>9.051792499119587</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>8.061792499119528</v>
+        <v>8.061792499119594</v>
       </c>
     </row>
     <row r="5">
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>8.558649048076902</v>
+        <v>8.558649048077335</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>8.061792499119449</v>
+        <v>8.061792499119676</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>9.051792499119539</v>
+        <v>9.05179249911961</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>8.061792499119546</v>
+        <v>8.061792499119523</v>
       </c>
     </row>
     <row r="7">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>7.634999038461534</v>
+        <v>7.63499903846186</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>8.061792499119568</v>
+        <v>8.061792499119537</v>
       </c>
     </row>
     <row r="8">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>9.051792499119575</v>
+        <v>9.051792499119628</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -723,7 +723,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>8.06179249911953</v>
+        <v>8.061792499119637</v>
       </c>
     </row>
     <row r="9">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>6.702019230769267</v>
+        <v>6.702019230769403</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>8.061792499119505</v>
+        <v>8.061792499119687</v>
       </c>
     </row>
     <row r="10">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>9.051792499119566</v>
+        <v>9.051792499119578</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>8.06179249911958</v>
+        <v>8.061792499119599</v>
       </c>
     </row>
     <row r="11">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>5.759615384615401</v>
+        <v>5.759615384615515</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>7.555672969608564</v>
+        <v>7.555672969608658</v>
       </c>
     </row>
     <row r="12">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>8.061792499119544</v>
+        <v>8.061792499119562</v>
       </c>
     </row>
     <row r="13">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>4.807692307692323</v>
+        <v>4.80769230769242</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>6.626942393543905</v>
+        <v>6.626942393544043</v>
       </c>
     </row>
     <row r="14">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>9.051792499119511</v>
+        <v>9.051792499119678</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>8.061792499119509</v>
+        <v>8.061792499119623</v>
       </c>
     </row>
     <row r="15">
@@ -963,7 +963,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>4.807692307692314</v>
+        <v>4.807692307692474</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>6.626942393543909</v>
+        <v>6.626942393544674</v>
       </c>
     </row>
     <row r="16">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>9.051792499119571</v>
+        <v>9.05179249911957</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>8.061792499119534</v>
+        <v>8.061792499119575</v>
       </c>
     </row>
     <row r="17">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>4.807692307692321</v>
+        <v>4.807692307692497</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>6.626942393543999</v>
+        <v>6.626942393544084</v>
       </c>
     </row>
     <row r="18">
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>9.051792499119522</v>
+        <v>9.05179249911957</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>8.061792499119569</v>
+        <v>8.061792499119589</v>
       </c>
     </row>
     <row r="19">
@@ -1111,7 +1111,7 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>4.807692307692317</v>
+        <v>4.807692307692397</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>6.626942393543889</v>
+        <v>6.626942393544589</v>
       </c>
     </row>
     <row r="20">
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>9.051792499119546</v>
+        <v>9.05179249911957</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>8.061792499119544</v>
+        <v>8.061792499119576</v>
       </c>
     </row>
     <row r="21">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>4.807692307692303</v>
+        <v>4.807692307692388</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>6.626942393543891</v>
+        <v>6.626942393544339</v>
       </c>
     </row>
     <row r="22">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>9.051792499119601</v>
+        <v>9.051792499119617</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>8.061792499119584</v>
+        <v>8.061792499119546</v>
       </c>
     </row>
     <row r="23">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>4.807692307692291</v>
+        <v>4.807692307692302</v>
       </c>
       <c r="I23" t="n">
         <v>1</v>
@@ -1278,7 +1278,7 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>6.626942393543899</v>
+        <v>6.626942393544745</v>
       </c>
     </row>
     <row r="24">
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>7.57179249911956</v>
+        <v>7.571792499119557</v>
       </c>
     </row>
     <row r="25">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>7.571792499119552</v>
+        <v>7.57179249911958</v>
       </c>
     </row>
     <row r="26">
@@ -1341,7 +1341,7 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>7.571792499119611</v>
+        <v>7.571792499119528</v>
       </c>
     </row>
     <row r="27">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>7.571792499119629</v>
+        <v>7.571792499119633</v>
       </c>
     </row>
     <row r="28">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>7.571792499119596</v>
+        <v>7.57179249911967</v>
       </c>
     </row>
     <row r="29">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>7.571792499119534</v>
+        <v>7.571792499119567</v>
       </c>
     </row>
     <row r="30">
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>7.571792499119538</v>
+        <v>7.571792499119598</v>
       </c>
     </row>
     <row r="31">
@@ -1446,7 +1446,7 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>7.480116239912532</v>
+        <v>7.480116239912875</v>
       </c>
     </row>
     <row r="32">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>7.571792499119583</v>
+        <v>7.571792499119605</v>
       </c>
     </row>
     <row r="33">
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>6.560672969608485</v>
+        <v>6.560672969608582</v>
       </c>
     </row>
     <row r="34">
@@ -1509,7 +1509,7 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>7.183057116715489</v>
+        <v>7.183057116715496</v>
       </c>
     </row>
     <row r="35">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>5.248538375686806</v>
+        <v>5.248538375687652</v>
       </c>
     </row>
     <row r="36">
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>7.183057116715451</v>
+        <v>7.183057116715597</v>
       </c>
     </row>
     <row r="37">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>5.248538375686874</v>
+        <v>5.248538375686914</v>
       </c>
     </row>
     <row r="38">
@@ -1593,7 +1593,7 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>7.183057116715551</v>
+        <v>7.183057116715641</v>
       </c>
     </row>
     <row r="39">
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>5.248538375686795</v>
+        <v>5.248538375687275</v>
       </c>
     </row>
     <row r="40">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>7.183057116715513</v>
+        <v>7.183057116715517</v>
       </c>
     </row>
     <row r="41">
@@ -1656,7 +1656,7 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>5.248538375686802</v>
+        <v>5.248538375687016</v>
       </c>
     </row>
     <row r="42">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>7.183057116715619</v>
+        <v>7.183057116715606</v>
       </c>
     </row>
     <row r="43">
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>5.248538375686765</v>
+        <v>5.248538375687566</v>
       </c>
     </row>
     <row r="44">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>7.183057116715553</v>
+        <v>7.183057116715468</v>
       </c>
     </row>
     <row r="45">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>5.248538375686779</v>
+        <v>5.248538375687385</v>
       </c>
     </row>
     <row r="46">
@@ -1761,7 +1761,7 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>6.591692499119505</v>
+        <v>6.591692499119581</v>
       </c>
     </row>
     <row r="47">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>6.591692499119581</v>
+        <v>6.591692499119544</v>
       </c>
     </row>
     <row r="48">
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>6.591692499119565</v>
+        <v>6.591692499119572</v>
       </c>
     </row>
     <row r="49">
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>6.591692499119578</v>
+        <v>6.59169249911961</v>
       </c>
     </row>
     <row r="51">
@@ -1866,7 +1866,7 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>6.591692499119455</v>
+        <v>6.591692499119699</v>
       </c>
     </row>
     <row r="52">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>6.591692499119551</v>
+        <v>6.591692499119591</v>
       </c>
     </row>
     <row r="53">
@@ -1908,7 +1908,7 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>6.495066239912524</v>
+        <v>6.495066239912563</v>
       </c>
     </row>
     <row r="54">
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>6.591692499119526</v>
+        <v>6.591692499119535</v>
       </c>
     </row>
     <row r="55">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>5.196052991929886</v>
+        <v>5.196052991931087</v>
       </c>
     </row>
     <row r="56">
@@ -1971,7 +1971,7 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>6.400103890993475</v>
+        <v>6.400103890993799</v>
       </c>
     </row>
     <row r="57">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>4.156842393543997</v>
+        <v>4.156842393544268</v>
       </c>
     </row>
     <row r="58">
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>6.400103890993378</v>
+        <v>6.400103890993684</v>
       </c>
     </row>
     <row r="59">
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>4.156842393543835</v>
+        <v>4.156842393544569</v>
       </c>
     </row>
     <row r="60">
@@ -2055,7 +2055,7 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>6.400103890993416</v>
+        <v>6.400103890993682</v>
       </c>
     </row>
     <row r="61">
@@ -2076,7 +2076,7 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>4.156842393543871</v>
+        <v>4.156842393544416</v>
       </c>
     </row>
     <row r="62">
@@ -2097,7 +2097,7 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>6.400103890993631</v>
+        <v>6.400103890993736</v>
       </c>
     </row>
     <row r="63">
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>4.15684239354383</v>
+        <v>4.156842393544709</v>
       </c>
     </row>
     <row r="64">
@@ -2139,7 +2139,7 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>6.400103890993688</v>
+        <v>6.400103890993515</v>
       </c>
     </row>
     <row r="65">
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>4.156842393543882</v>
+        <v>4.156842393544524</v>
       </c>
     </row>
     <row r="66">
@@ -2181,7 +2181,7 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>6.400103890993614</v>
+        <v>6.400103890993543</v>
       </c>
     </row>
     <row r="67">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>4.156842393543883</v>
+        <v>4.156842393544534</v>
       </c>
     </row>
     <row r="68">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>5.621393499119566</v>
+        <v>5.621393499119616</v>
       </c>
     </row>
     <row r="69">
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>5.621393499119574</v>
+        <v>5.621393499119595</v>
       </c>
     </row>
     <row r="70">
@@ -2265,7 +2265,7 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>5.621393499119553</v>
+        <v>5.621393499119573</v>
       </c>
     </row>
     <row r="71">
@@ -2286,7 +2286,7 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>5.621393499119553</v>
+        <v>5.621393499119706</v>
       </c>
     </row>
     <row r="72">
@@ -2307,7 +2307,7 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>5.621393499119567</v>
+        <v>5.621393499119585</v>
       </c>
     </row>
     <row r="73">
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>5.621393499119648</v>
+        <v>5.621393499119545</v>
       </c>
     </row>
     <row r="74">
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>5.621393499119553</v>
+        <v>5.621393499119591</v>
       </c>
     </row>
     <row r="75">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>5.144092462010455</v>
+        <v>5.144092462011854</v>
       </c>
     </row>
     <row r="76">
@@ -2391,7 +2391,7 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>5.621393499119517</v>
+        <v>5.621393499119613</v>
       </c>
     </row>
     <row r="77">
@@ -2412,7 +2412,7 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>4.115273969608582</v>
+        <v>4.115273969608971</v>
       </c>
     </row>
     <row r="78">
@@ -2433,7 +2433,7 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>5.621393499119586</v>
+        <v>5.621393499119593</v>
       </c>
     </row>
     <row r="79">
@@ -2454,7 +2454,7 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>3.292219175686729</v>
+        <v>3.292219175687312</v>
       </c>
     </row>
     <row r="80">
@@ -2475,7 +2475,7 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>5.621393499119536</v>
+        <v>5.621393499119552</v>
       </c>
     </row>
     <row r="81">
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>3.292219175686726</v>
+        <v>3.292219175687187</v>
       </c>
     </row>
     <row r="82">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>5.621393499119549</v>
+        <v>5.621393499119621</v>
       </c>
     </row>
     <row r="83">
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>3.292219175686642</v>
+        <v>3.29221917568748</v>
       </c>
     </row>
     <row r="84">
@@ -2559,7 +2559,7 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>5.621393499119542</v>
+        <v>5.621393499119628</v>
       </c>
     </row>
     <row r="85">
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>3.292219175686784</v>
+        <v>3.292219175687272</v>
       </c>
     </row>
     <row r="86">
@@ -2601,7 +2601,7 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>5.621393499119552</v>
+        <v>5.621393499119601</v>
       </c>
     </row>
     <row r="87">
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>3.292219175686719</v>
+        <v>3.292219175687492</v>
       </c>
     </row>
     <row r="88">
@@ -2643,7 +2643,7 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>5.621393499119518</v>
+        <v>5.621393499119538</v>
       </c>
     </row>
     <row r="89">
@@ -2664,7 +2664,7 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>3.292219175686757</v>
+        <v>3.292219175687267</v>
       </c>
     </row>
     <row r="90">
@@ -2685,7 +2685,7 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>4.660797489119532</v>
+        <v>4.660797489119582</v>
       </c>
     </row>
     <row r="91">
@@ -2706,7 +2706,7 @@
         </is>
       </c>
       <c r="M91" t="n">
-        <v>4.66079748911951</v>
+        <v>4.66079748911959</v>
       </c>
     </row>
     <row r="92">
@@ -2727,7 +2727,7 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>4.660797489119561</v>
+        <v>4.660797489119608</v>
       </c>
     </row>
     <row r="93">
@@ -2748,7 +2748,7 @@
         </is>
       </c>
       <c r="M93" t="n">
-        <v>4.660797489119538</v>
+        <v>4.660797489119609</v>
       </c>
     </row>
     <row r="94">
@@ -2769,7 +2769,7 @@
         </is>
       </c>
       <c r="M94" t="n">
-        <v>4.660797489119562</v>
+        <v>4.66079748911962</v>
       </c>
     </row>
     <row r="95">
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="M95" t="n">
-        <v>4.660797489119627</v>
+        <v>4.660797489119634</v>
       </c>
     </row>
     <row r="96">
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="M96" t="n">
-        <v>4.660797489119638</v>
+        <v>4.660797489119643</v>
       </c>
     </row>
     <row r="97">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="M97" t="n">
-        <v>4.074121229912435</v>
+        <v>4.074121229912832</v>
       </c>
     </row>
     <row r="98">
@@ -2853,7 +2853,7 @@
         </is>
       </c>
       <c r="M98" t="n">
-        <v>4.660797489119612</v>
+        <v>4.660797489119608</v>
       </c>
     </row>
     <row r="99">
@@ -2874,7 +2874,7 @@
         </is>
       </c>
       <c r="M99" t="n">
-        <v>3.259296983929928</v>
+        <v>3.259296983930386</v>
       </c>
     </row>
     <row r="100">
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="M100" t="n">
-        <v>4.66079748911954</v>
+        <v>4.660797489119602</v>
       </c>
     </row>
     <row r="101">
@@ -2916,7 +2916,7 @@
         </is>
       </c>
       <c r="M101" t="n">
-        <v>2.607437587143834</v>
+        <v>2.607437587144193</v>
       </c>
     </row>
     <row r="102">
@@ -2937,7 +2937,7 @@
         </is>
       </c>
       <c r="M102" t="n">
-        <v>4.66079748911956</v>
+        <v>4.660797489119614</v>
       </c>
     </row>
     <row r="103">
@@ -2958,7 +2958,7 @@
         </is>
       </c>
       <c r="M103" t="n">
-        <v>2.607437587143786</v>
+        <v>2.607437587144704</v>
       </c>
     </row>
     <row r="104">
@@ -2979,7 +2979,7 @@
         </is>
       </c>
       <c r="M104" t="n">
-        <v>4.660797489119582</v>
+        <v>4.660797489119641</v>
       </c>
     </row>
     <row r="105">
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="M105" t="n">
-        <v>2.607437587143927</v>
+        <v>2.60743758714437</v>
       </c>
     </row>
     <row r="106">
@@ -3021,7 +3021,7 @@
         </is>
       </c>
       <c r="M106" t="n">
-        <v>4.660797489119529</v>
+        <v>4.660797489119564</v>
       </c>
     </row>
     <row r="107">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="M107" t="n">
-        <v>2.607437587143844</v>
+        <v>2.60743758714456</v>
       </c>
     </row>
     <row r="108">
@@ -3063,7 +3063,7 @@
         </is>
       </c>
       <c r="M108" t="n">
-        <v>4.660797489119567</v>
+        <v>4.660797489119521</v>
       </c>
     </row>
     <row r="109">
@@ -3084,7 +3084,7 @@
         </is>
       </c>
       <c r="M109" t="n">
-        <v>2.607437587143965</v>
+        <v>2.607437587144574</v>
       </c>
     </row>
     <row r="110">
@@ -3105,7 +3105,7 @@
         </is>
       </c>
       <c r="M110" t="n">
-        <v>4.660797489119572</v>
+        <v>4.660797489119645</v>
       </c>
     </row>
     <row r="111">
@@ -3126,7 +3126,7 @@
         </is>
       </c>
       <c r="M111" t="n">
-        <v>2.607437587143912</v>
+        <v>2.607437587144369</v>
       </c>
     </row>
     <row r="112">
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="M112" t="n">
-        <v>3.709807439219522</v>
+        <v>3.709807439219601</v>
       </c>
     </row>
     <row r="113">
@@ -3168,7 +3168,7 @@
         </is>
       </c>
       <c r="M113" t="n">
-        <v>3.70980743921958</v>
+        <v>3.709807439219567</v>
       </c>
     </row>
     <row r="114">
@@ -3189,7 +3189,7 @@
         </is>
       </c>
       <c r="M114" t="n">
-        <v>3.709807439219508</v>
+        <v>3.709807439219516</v>
       </c>
     </row>
     <row r="115">
@@ -3210,7 +3210,7 @@
         </is>
       </c>
       <c r="M115" t="n">
-        <v>3.709807439219404</v>
+        <v>3.709807439219598</v>
       </c>
     </row>
     <row r="116">
@@ -3231,7 +3231,7 @@
         </is>
       </c>
       <c r="M116" t="n">
-        <v>3.709807439219516</v>
+        <v>3.709807439219551</v>
       </c>
     </row>
     <row r="117">
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="M117" t="n">
-        <v>3.709807439219647</v>
+        <v>3.709807439219596</v>
       </c>
     </row>
     <row r="118">
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="M118" t="n">
-        <v>3.709807439219528</v>
+        <v>3.70980743921961</v>
       </c>
     </row>
     <row r="119">
@@ -3294,7 +3294,7 @@
         </is>
       </c>
       <c r="M119" t="n">
-        <v>3.226704014090821</v>
+        <v>3.226704014091368</v>
       </c>
     </row>
     <row r="120">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="M120" t="n">
-        <v>3.709807439219539</v>
+        <v>3.709807439219603</v>
       </c>
     </row>
     <row r="121">
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="M121" t="n">
-        <v>2.581363211272397</v>
+        <v>2.581363211272919</v>
       </c>
     </row>
     <row r="122">
@@ -3357,7 +3357,7 @@
         </is>
       </c>
       <c r="M122" t="n">
-        <v>3.709807439219572</v>
+        <v>3.709807439219562</v>
       </c>
     </row>
     <row r="123">
@@ -3378,7 +3378,7 @@
         </is>
       </c>
       <c r="M123" t="n">
-        <v>2.065090569017858</v>
+        <v>2.065090569018649</v>
       </c>
     </row>
     <row r="124">
@@ -3399,7 +3399,7 @@
         </is>
       </c>
       <c r="M124" t="n">
-        <v>3.709807439219574</v>
+        <v>3.709807439219538</v>
       </c>
     </row>
     <row r="125">
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="M125" t="n">
-        <v>2.065090569018031</v>
+        <v>2.065090569018387</v>
       </c>
     </row>
     <row r="126">
@@ -3441,7 +3441,7 @@
         </is>
       </c>
       <c r="M126" t="n">
-        <v>3.709807439219547</v>
+        <v>3.709807439219635</v>
       </c>
     </row>
     <row r="127">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="M127" t="n">
-        <v>2.065090569017916</v>
+        <v>2.065090569018499</v>
       </c>
     </row>
     <row r="128">
@@ -3483,7 +3483,7 @@
         </is>
       </c>
       <c r="M128" t="n">
-        <v>3.709807439219572</v>
+        <v>3.709807439219578</v>
       </c>
     </row>
     <row r="129">
@@ -3504,7 +3504,7 @@
         </is>
       </c>
       <c r="M129" t="n">
-        <v>2.065090569017951</v>
+        <v>2.065090569018597</v>
       </c>
     </row>
     <row r="130">
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="M130" t="n">
-        <v>3.709807439219546</v>
+        <v>3.70980743921957</v>
       </c>
     </row>
     <row r="131">
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="M131" t="n">
-        <v>2.065090569017949</v>
+        <v>2.065090569018494</v>
       </c>
     </row>
     <row r="132">
@@ -3567,7 +3567,7 @@
         </is>
       </c>
       <c r="M132" t="n">
-        <v>3.709807439219597</v>
+        <v>3.709807439219543</v>
       </c>
     </row>
     <row r="133">
@@ -3588,7 +3588,7 @@
         </is>
       </c>
       <c r="M133" t="n">
-        <v>2.065090569018007</v>
+        <v>2.065090569018452</v>
       </c>
     </row>
     <row r="134">
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="M134" t="n">
-        <v>2.768327289818535</v>
+        <v>2.768327289818607</v>
       </c>
     </row>
     <row r="135">
@@ -3630,7 +3630,7 @@
         </is>
       </c>
       <c r="M135" t="n">
-        <v>2.768327289818528</v>
+        <v>2.768327289818726</v>
       </c>
     </row>
     <row r="136">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="M136" t="n">
-        <v>2.76832728981856</v>
+        <v>2.768327289818534</v>
       </c>
     </row>
     <row r="137">
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="M137" t="n">
-        <v>2.768327289818522</v>
+        <v>2.768327289818667</v>
       </c>
     </row>
     <row r="138">
@@ -3693,7 +3693,7 @@
         </is>
       </c>
       <c r="M138" t="n">
-        <v>2.768327289818614</v>
+        <v>2.768327289818568</v>
       </c>
     </row>
     <row r="139">
@@ -3714,7 +3714,7 @@
         </is>
       </c>
       <c r="M139" t="n">
-        <v>2.76832728981854</v>
+        <v>2.768327289818494</v>
       </c>
     </row>
     <row r="140">
@@ -3735,7 +3735,7 @@
         </is>
       </c>
       <c r="M140" t="n">
-        <v>2.768327289818574</v>
+        <v>2.768327289818552</v>
       </c>
     </row>
     <row r="141">
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="M141" t="n">
-        <v>2.555549579159661</v>
+        <v>2.555549579160356</v>
       </c>
     </row>
     <row r="142">
@@ -3777,7 +3777,7 @@
         </is>
       </c>
       <c r="M142" t="n">
-        <v>2.768327289818524</v>
+        <v>2.768327289818594</v>
       </c>
     </row>
     <row r="143">
@@ -3798,7 +3798,7 @@
         </is>
       </c>
       <c r="M143" t="n">
-        <v>2.044439663327437</v>
+        <v>2.044439663328554</v>
       </c>
     </row>
     <row r="144">
@@ -3819,7 +3819,7 @@
         </is>
       </c>
       <c r="M144" t="n">
-        <v>2.768327289818551</v>
+        <v>2.768327289818595</v>
       </c>
     </row>
     <row r="145">
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="M145" t="n">
-        <v>1.635551730662203</v>
+        <v>1.635551730662662</v>
       </c>
     </row>
     <row r="146">
@@ -3861,7 +3861,7 @@
         </is>
       </c>
       <c r="M146" t="n">
-        <v>2.768327289818588</v>
+        <v>2.768327289818544</v>
       </c>
     </row>
     <row r="147">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="M147" t="n">
-        <v>1.635551730662112</v>
+        <v>1.635551730662666</v>
       </c>
     </row>
     <row r="148">
@@ -3903,7 +3903,7 @@
         </is>
       </c>
       <c r="M148" t="n">
-        <v>2.76832728981856</v>
+        <v>2.768327289818633</v>
       </c>
     </row>
     <row r="149">
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="M149" t="n">
-        <v>1.635551730662246</v>
+        <v>1.635551730662795</v>
       </c>
     </row>
     <row r="150">
@@ -3945,7 +3945,7 @@
         </is>
       </c>
       <c r="M150" t="n">
-        <v>2.768327289818533</v>
+        <v>2.768327289818551</v>
       </c>
     </row>
     <row r="151">
@@ -3966,7 +3966,7 @@
         </is>
       </c>
       <c r="M151" t="n">
-        <v>1.635551730662293</v>
+        <v>1.635551730662797</v>
       </c>
     </row>
     <row r="152">
@@ -3987,7 +3987,7 @@
         </is>
       </c>
       <c r="M152" t="n">
-        <v>2.76832728981856</v>
+        <v>2.768327289818683</v>
       </c>
     </row>
     <row r="153">
@@ -4008,7 +4008,7 @@
         </is>
       </c>
       <c r="M153" t="n">
-        <v>1.635551730662233</v>
+        <v>1.6355517306626</v>
       </c>
     </row>
     <row r="154">
@@ -4029,7 +4029,7 @@
         </is>
       </c>
       <c r="M154" t="n">
-        <v>2.76832728981858</v>
+        <v>2.768327289818576</v>
       </c>
     </row>
     <row r="155">
@@ -4050,7 +4050,7 @@
         </is>
       </c>
       <c r="M155" t="n">
-        <v>1.63555173066222</v>
+        <v>1.635551730662655</v>
       </c>
     </row>
     <row r="156">
@@ -4071,7 +4071,7 @@
         </is>
       </c>
       <c r="M156" t="n">
-        <v>1.83626194191158</v>
+        <v>1.83626194191159</v>
       </c>
     </row>
     <row r="157">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="M157" t="n">
-        <v>1.836261941911592</v>
+        <v>1.836261941911552</v>
       </c>
     </row>
     <row r="158">
@@ -4113,7 +4113,7 @@
         </is>
       </c>
       <c r="M158" t="n">
-        <v>1.836261941911621</v>
+        <v>1.836261941911583</v>
       </c>
     </row>
     <row r="159">
@@ -4134,7 +4134,7 @@
         </is>
       </c>
       <c r="M159" t="n">
-        <v>1.836261941911572</v>
+        <v>1.836261941911658</v>
       </c>
     </row>
     <row r="160">
@@ -4155,7 +4155,7 @@
         </is>
       </c>
       <c r="M160" t="n">
-        <v>1.836261941911544</v>
+        <v>1.836261941911618</v>
       </c>
     </row>
     <row r="161">
@@ -4176,7 +4176,7 @@
         </is>
       </c>
       <c r="M161" t="n">
-        <v>1.836261941911481</v>
+        <v>1.836261941911669</v>
       </c>
     </row>
     <row r="162">
@@ -4197,7 +4197,7 @@
         </is>
       </c>
       <c r="M162" t="n">
-        <v>1.836261941911547</v>
+        <v>1.836261941911659</v>
       </c>
     </row>
     <row r="163">
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="M163" t="n">
-        <v>1.836261941911542</v>
+        <v>1.836261941911617</v>
       </c>
     </row>
     <row r="164">
@@ -4239,7 +4239,7 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>1.836261941911573</v>
+        <v>1.836261941911588</v>
       </c>
     </row>
     <row r="165">
@@ -4260,7 +4260,7 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>1.619196213355571</v>
+        <v>1.619196213356137</v>
       </c>
     </row>
     <row r="166">
@@ -4281,7 +4281,7 @@
         </is>
       </c>
       <c r="M166" t="n">
-        <v>1.836261941911555</v>
+        <v>1.836261941911603</v>
       </c>
     </row>
     <row r="167">
@@ -4302,7 +4302,7 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>1.29535697068418</v>
+        <v>1.295356970684954</v>
       </c>
     </row>
     <row r="168">
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="M168" t="n">
-        <v>1.836261941911542</v>
+        <v>1.836261941911579</v>
       </c>
     </row>
     <row r="169">
@@ -4344,7 +4344,7 @@
         </is>
       </c>
       <c r="M169" t="n">
-        <v>1.295356970684623</v>
+        <v>1.295356970684887</v>
       </c>
     </row>
     <row r="170">
@@ -4365,7 +4365,7 @@
         </is>
       </c>
       <c r="M170" t="n">
-        <v>1.83626194191155</v>
+        <v>1.836261941911658</v>
       </c>
     </row>
     <row r="171">
@@ -4386,7 +4386,7 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>1.295356970684397</v>
+        <v>1.295356970685277</v>
       </c>
     </row>
     <row r="172">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="M172" t="n">
-        <v>1.836261941911639</v>
+        <v>1.836261941911636</v>
       </c>
     </row>
     <row r="173">
@@ -4428,7 +4428,7 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>1.295356970684508</v>
+        <v>1.295356970684793</v>
       </c>
     </row>
     <row r="174">
@@ -4449,7 +4449,7 @@
         </is>
       </c>
       <c r="M174" t="n">
-        <v>1.836261941911601</v>
+        <v>1.836261941911583</v>
       </c>
     </row>
     <row r="175">
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="M175" t="n">
-        <v>1.295356970684485</v>
+        <v>1.295356970684937</v>
       </c>
     </row>
     <row r="176">
@@ -4491,7 +4491,7 @@
         </is>
       </c>
       <c r="M176" t="n">
-        <v>1.836261941911566</v>
+        <v>1.836261941911665</v>
       </c>
     </row>
     <row r="177">
@@ -4512,7 +4512,7 @@
         </is>
       </c>
       <c r="M177" t="n">
-        <v>1.295356970684545</v>
+        <v>1.295356970684959</v>
       </c>
     </row>
     <row r="178">
@@ -4533,7 +4533,7 @@
         </is>
       </c>
       <c r="M178" t="n">
-        <v>0.9135172474836375</v>
+        <v>0.9135172474836466</v>
       </c>
     </row>
     <row r="179">
@@ -4554,7 +4554,7 @@
         </is>
       </c>
       <c r="M179" t="n">
-        <v>0.9135172474836342</v>
+        <v>0.9135172474836453</v>
       </c>
     </row>
     <row r="180">
@@ -4575,7 +4575,7 @@
         </is>
       </c>
       <c r="M180" t="n">
-        <v>0.9135172474836297</v>
+        <v>0.9135172474836821</v>
       </c>
     </row>
     <row r="181">
@@ -4596,7 +4596,7 @@
         </is>
       </c>
       <c r="M181" t="n">
-        <v>0.9135172474836792</v>
+        <v>0.9135172474836519</v>
       </c>
     </row>
     <row r="182">
@@ -4617,7 +4617,7 @@
         </is>
       </c>
       <c r="M182" t="n">
-        <v>0.9135172474836599</v>
+        <v>0.9135172474836082</v>
       </c>
     </row>
     <row r="183">
@@ -4638,7 +4638,7 @@
         </is>
       </c>
       <c r="M183" t="n">
-        <v>0.913517247483604</v>
+        <v>0.913517247483842</v>
       </c>
     </row>
     <row r="184">
@@ -4659,7 +4659,7 @@
         </is>
       </c>
       <c r="M184" t="n">
-        <v>0.9135172474836573</v>
+        <v>0.913517247483675</v>
       </c>
     </row>
     <row r="185">
@@ -4680,7 +4680,7 @@
         </is>
       </c>
       <c r="M185" t="n">
-        <v>0.9135172474836533</v>
+        <v>0.9135172474837221</v>
       </c>
     </row>
     <row r="186">
@@ -4701,7 +4701,7 @@
         </is>
       </c>
       <c r="M186" t="n">
-        <v>0.9135172474836484</v>
+        <v>0.9135172474836473</v>
       </c>
     </row>
     <row r="187">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="M187" t="n">
-        <v>0.9135172474835989</v>
+        <v>0.9135172474836397</v>
       </c>
     </row>
     <row r="188">
@@ -4743,7 +4743,7 @@
         </is>
       </c>
       <c r="M188" t="n">
-        <v>0.9135172474836588</v>
+        <v>0.9135172474836333</v>
       </c>
     </row>
     <row r="189">
@@ -4764,7 +4764,7 @@
         </is>
       </c>
       <c r="M189" t="n">
-        <v>0.9135172474836817</v>
+        <v>0.913517247483804</v>
       </c>
     </row>
     <row r="190">
@@ -4785,7 +4785,7 @@
         </is>
       </c>
       <c r="M190" t="n">
-        <v>0.9135172474837298</v>
+        <v>0.9135172474836479</v>
       </c>
     </row>
     <row r="191">
@@ -4806,7 +4806,7 @@
         </is>
       </c>
       <c r="M191" t="n">
-        <v>0.913517247483643</v>
+        <v>0.9135172474836741</v>
       </c>
     </row>
     <row r="192">
@@ -4827,7 +4827,7 @@
         </is>
       </c>
       <c r="M192" t="n">
-        <v>0.9135172474836427</v>
+        <v>0.9135172474836426</v>
       </c>
     </row>
     <row r="193">
@@ -4848,7 +4848,7 @@
         </is>
       </c>
       <c r="M193" t="n">
-        <v>0.9135172474836446</v>
+        <v>0.9135172474835751</v>
       </c>
     </row>
     <row r="194">
@@ -4869,7 +4869,7 @@
         </is>
       </c>
       <c r="M194" t="n">
-        <v>0.9135172474836204</v>
+        <v>0.9135172474836439</v>
       </c>
     </row>
     <row r="195">
@@ -4890,7 +4890,7 @@
         </is>
       </c>
       <c r="M195" t="n">
-        <v>0.9135172474836137</v>
+        <v>0.9135172474836839</v>
       </c>
     </row>
     <row r="196">
@@ -4911,7 +4911,7 @@
         </is>
       </c>
       <c r="M196" t="n">
-        <v>0.9135172474836699</v>
+        <v>0.9135172474836506</v>
       </c>
     </row>
     <row r="197">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="M197" t="n">
-        <v>0.9135172474836577</v>
+        <v>0.9135172474836371</v>
       </c>
     </row>
     <row r="198">
@@ -4953,7 +4953,7 @@
         </is>
       </c>
       <c r="M198" t="n">
-        <v>0.9135172474836417</v>
+        <v>0.9135172474837034</v>
       </c>
     </row>
     <row r="199">
@@ -4974,7 +4974,7 @@
         </is>
       </c>
       <c r="M199" t="n">
-        <v>0.9135172474835436</v>
+        <v>0.9135172474836911</v>
       </c>
     </row>
     <row r="200">

</xml_diff>